<commit_message>
Atualização automática de SANTA_ROSA.xlsx
</commit_message>
<xml_diff>
--- a/SANTA_ROSA.xlsx
+++ b/SANTA_ROSA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE507FD0-2AEA-4CA6-86F7-2E6EFB708FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0125927B-65F0-4D23-84AB-9B85DD95CAE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1235,7 +1235,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{BD065D67-0862-4690-81C9-7F76322A7157}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{4EF2C3F0-618B-4535-9637-74618CADF5AE}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1265,10 +1265,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE91F7BF-BEA0-4D62-BA59-20DC196DB83D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{756F25BA-A610-447E-928B-3053FA6715F9}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1306,7 +1306,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDD1D6EE-0007-4372-8472-5B71497BAF56}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E76D73AB-F057-4CA5-A482-14190189109E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1369,7 +1369,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55CC417C-DE8D-4B12-8F55-F122C554323D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A6031FE-CBD9-4A11-AFE6-352517E3DEBE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1388,7 +1388,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D6AC8F6-D391-A694-59CF-3E088EAFD36C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD47713A-BC5D-071E-BA8D-F0C59D64FD18}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1437,7 +1437,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A5A088D-C29A-7B3F-FB0C-C5B4BE5D7BD1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{074674C9-1AD1-ABEC-9CEB-32DDAF99F00C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1456,7 +1456,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C46361D0-86F1-6F50-6580-EC73C648364E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF7FB23F-B685-EDD5-4276-05E46A125A0A}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1487,7 +1487,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DD07872-B7C9-F898-9203-52A039D7FA62}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C175FCE-064A-981E-8088-E822C21F478A}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1518,7 +1518,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43274D48-5058-CA1C-90FB-AE1066FD5C03}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AFCDEE4-B9B2-594A-0D56-B3D2A107E5CD}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1561,7 +1561,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57982158-E769-42BA-8113-74C4DE8F12D2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB1E7081-85D3-4AF9-AC74-DAD840BA4E8E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1599,7 +1599,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF3C755E-0C34-425C-8AEA-8FC7242A4968}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A353170D-AEEB-4ED7-9548-0BF75EA688C8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1642,7 +1642,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FD3FCD3-4947-49F4-8823-FA020551D4CD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{769D9C34-F485-4C1A-A524-4FF5AEF6CC96}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1955,7 +1955,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52729E45-CFDD-490F-87B1-E4D8EA9B71F6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D36A0FF-4C44-4EDD-A622-6CA6AFA5E9AB}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>